<commit_message>
Completed Random Forest configuration testing.
</commit_message>
<xml_diff>
--- a/evidence/configurations.xlsx
+++ b/evidence/configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\F21DL-CW2\evidence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C66346-A5BF-41DD-8137-989B3BE34FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C6D40D-47C6-4DCC-AC23-705EB62D2FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7070" yWindow="4680" windowWidth="28800" windowHeight="13640" xr2:uid="{87CF2611-45DB-404B-9ED3-045615C6A122}"/>
+    <workbookView xWindow="-14610" yWindow="4550" windowWidth="28800" windowHeight="13640" activeTab="1" xr2:uid="{87CF2611-45DB-404B-9ED3-045615C6A122}"/>
   </bookViews>
   <sheets>
     <sheet name="J48" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Binary Splits</t>
   </si>
@@ -78,6 +78,18 @@
   <si>
     <t>NumIteration</t>
   </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Bag Size Percent</t>
+  </si>
+  <si>
+    <t>Max Depth</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,13 +171,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,13 +866,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>14654</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2761911</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1129812</xdr:rowOff>
@@ -890,14 +910,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>798287</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2747257</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2710972</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1120042</xdr:rowOff>
     </xdr:to>
@@ -922,7 +942,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3492500" y="1514231"/>
+          <a:off x="3447144" y="1324429"/>
           <a:ext cx="2747257" cy="1120042"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -934,13 +954,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2793127</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>947615</xdr:rowOff>
@@ -978,13 +998,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2793127</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>947615</xdr:rowOff>
@@ -1012,6 +1032,1238 @@
         <a:xfrm>
           <a:off x="3492500" y="3800231"/>
           <a:ext cx="2793127" cy="947615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2451393</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1092200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02E20FFB-5F39-4A81-BDDD-180AFD3C9844}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3486150" y="4756150"/>
+          <a:ext cx="2451393" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2511461</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1083235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A7F749D-406A-4AD2-BCDF-AF47CFA7E6B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3481294" y="5901765"/>
+          <a:ext cx="2511461" cy="1083235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2497804</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1106715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28FC5BA-2930-4C2B-9603-1F97D89637B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="7039430"/>
+          <a:ext cx="2497804" cy="1106714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2576285</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1135643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{778E2A6E-ACAE-4262-A192-DE44C0630C7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="8182430"/>
+          <a:ext cx="2576285" cy="1135642"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2576285</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1135643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5D42930-C8ED-4427-9E55-01688A2E6EEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="9325430"/>
+          <a:ext cx="2576285" cy="1135642"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2630714</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1135629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{849BCAE5-3A3F-4BE3-BE85-95B4077A2B85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="10468429"/>
+          <a:ext cx="2630714" cy="1135629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2703285</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>34127</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B220BE26-CDCE-4440-A827-BDDCF01E8B20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="11611429"/>
+          <a:ext cx="2703285" cy="1177127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2485571</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1112381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F5D5D8D-0BBB-47C8-B4BF-C07CBEF80D5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="12754430"/>
+          <a:ext cx="2485571" cy="1112380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2567215</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1142427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D84CCF-D018-4D6C-9328-AB73570D12E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483430" y="13897429"/>
+          <a:ext cx="2567214" cy="1142427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2602394</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1115785</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DFBAA12-5A91-4517-9D20-1E01253F6852}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3483429" y="15040429"/>
+          <a:ext cx="2602394" cy="1115785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2605422</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{527F1E22-FAA9-45C2-BEDB-96B53E9329B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="17145000"/>
+          <a:ext cx="2605422" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2528455</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1117435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E82DE4A-5AA7-4C6B-97AA-D31CD571A8C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="18288000"/>
+          <a:ext cx="2528455" cy="1117435"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2554449</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1133929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EBDFF20-189B-40ED-B4FC-8253D9196EE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987144" y="19431000"/>
+          <a:ext cx="2554448" cy="1133929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2431143</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1088433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D8720D-163B-4771-A4C6-EF05EFA83BE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="20574000"/>
+          <a:ext cx="2431143" cy="1088433"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22087</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>11043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2605476</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1130952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7AD56BD-DFA6-47C5-B15A-3862F9AEB4C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6029739" y="21728043"/>
+          <a:ext cx="2583389" cy="1119909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2603500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1127899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B56169C-1F2B-4CD2-8E0E-4B00206CAD9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6000750" y="22860001"/>
+          <a:ext cx="2603500" cy="1127898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2585357</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1130543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C82E3059-B541-4F04-979F-D42E07593899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="24003000"/>
+          <a:ext cx="2585357" cy="1130543"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2594428</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1133617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3420061-9773-4415-A512-1935696BEA48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="25146001"/>
+          <a:ext cx="2594428" cy="1133616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2612571</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1134011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF03937-249C-4FE8-A46D-162A8F123074}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="26289001"/>
+          <a:ext cx="2612571" cy="1134010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2676071</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>10131</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9549119F-5F4C-4095-9C98-2D1E17703001}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="27432000"/>
+          <a:ext cx="2676071" cy="1153131"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2661537</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1133929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05B6F212-3B96-4BD1-923A-FC14F9E9ABB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987144" y="28575000"/>
+          <a:ext cx="2661536" cy="1133929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>477</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B28286EC-3A1B-4854-BE5D-3C81D7E38373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987143" y="29718001"/>
+          <a:ext cx="2667000" cy="1143476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2540001</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1104783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E19C198-7D34-4D2C-BB89-7A3BAE22BE93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026728" y="26289001"/>
+          <a:ext cx="2540000" cy="1104782"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2575326</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1085273</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86964DCF-725B-48EF-9655-06F380C76016}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="28575000"/>
+          <a:ext cx="2575326" cy="1085273"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2563091</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1110127</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4DE45BB-32B9-4DCD-A56E-9AF8BDFA6A7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="29718001"/>
+          <a:ext cx="2563091" cy="1110126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2561431</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1096818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF02EF63-C10F-4972-AE51-E88E3D677EC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="27432000"/>
+          <a:ext cx="2561431" cy="1096818"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2643909</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1118189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6913A273-FAD5-4257-935B-43B2A50226E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="30861001"/>
+          <a:ext cx="2643909" cy="1118188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2597728</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1134033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1395467D-7809-43F8-95CA-E397CFF87521}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026727" y="26289000"/>
+          <a:ext cx="2597728" cy="1134033"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1322,7 +2574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC4369C-A14A-4F6C-9BC2-320B38543A4C}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1864,25 +3116,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BB2B9A-1435-4A52-9948-1AEE37B4D992}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.36328125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.36328125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.54296875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1890,31 +3144,40 @@
         <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="b">
         <v>0</v>
       </c>
@@ -1924,27 +3187,35 @@
       <c r="C2" s="5">
         <v>100</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2">
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>100</v>
+      </c>
+      <c r="H2" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F2" s="2">
+      <c r="I2" s="7">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="J2" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H2" s="2">
+      <c r="K2" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="I2" s="2">
+      <c r="L2" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="J2" s="2">
+      <c r="M2" s="7">
         <v>0.995</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="b">
         <v>1</v>
       </c>
@@ -1954,27 +3225,35 @@
       <c r="C3" s="5">
         <v>100</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>100</v>
+      </c>
+      <c r="H3" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F3" s="2">
+      <c r="I3" s="7">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="J3" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H3" s="2">
+      <c r="K3" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="I3" s="2">
+      <c r="L3" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="J3" s="2">
+      <c r="M3" s="7">
         <v>0.995</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="b">
         <v>0</v>
       </c>
@@ -1984,27 +3263,35 @@
       <c r="C4" s="5">
         <v>100</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>100</v>
+      </c>
+      <c r="H4" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F4" s="2">
+      <c r="I4" s="7">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="J4" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H4" s="2">
+      <c r="K4" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="I4" s="2">
+      <c r="L4" s="7">
         <v>0.92700000000000005</v>
       </c>
-      <c r="J4" s="2">
+      <c r="M4" s="7">
         <v>0.995</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="b">
         <v>1</v>
       </c>
@@ -2014,27 +3301,35 @@
       <c r="C5" s="5">
         <v>100</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>100</v>
+      </c>
+      <c r="H5" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F5" s="2">
+      <c r="I5" s="7">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="J5" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H5" s="2">
+      <c r="K5" s="7">
         <v>0.92800000000000005</v>
       </c>
-      <c r="I5" s="2">
+      <c r="L5" s="7">
         <v>0.92700000000000005</v>
       </c>
-      <c r="J5" s="2">
+      <c r="M5" s="7">
         <v>0.995</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="b">
         <v>0</v>
       </c>
@@ -2044,15 +3339,35 @@
       <c r="C6" s="5">
         <v>100</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>100</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="b">
         <v>1</v>
       </c>
@@ -2062,15 +3377,35 @@
       <c r="C7" s="5">
         <v>100</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>100</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="b">
         <v>0</v>
       </c>
@@ -2078,35 +3413,75 @@
         <v>5</v>
       </c>
       <c r="C8" s="5">
+        <v>100</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
         <v>50</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
         <v>5</v>
       </c>
       <c r="C9" s="5">
-        <v>50</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>25</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="b">
         <v>0</v>
       </c>
@@ -2114,35 +3489,75 @@
         <v>5</v>
       </c>
       <c r="C10" s="5">
-        <v>150</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>15</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5">
-        <v>150</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I11" s="7">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="b">
         <v>0</v>
       </c>
@@ -2150,18 +3565,837 @@
         <v>5</v>
       </c>
       <c r="C12" s="5">
+        <v>100</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="I12" s="7">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>100</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>150</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>100</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
         <v>200</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="H14" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5">
+        <v>100</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>250</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>80</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>100</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5">
+        <v>30</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>100</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="I18" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="L18" s="7">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="M18" s="7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>100</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I19" s="7">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>100</v>
+      </c>
+      <c r="D20" s="5">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>100</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>100</v>
+      </c>
+      <c r="D21" s="5">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>100</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I21" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>100</v>
+      </c>
+      <c r="D22" s="5">
+        <v>90</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>100</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="K22" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="M22" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>100</v>
+      </c>
+      <c r="D23" s="5">
+        <v>160</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>100</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I23" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K23" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L23" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>100</v>
+      </c>
+      <c r="D24" s="5">
+        <v>160</v>
+      </c>
+      <c r="E24" s="5">
+        <v>3</v>
+      </c>
+      <c r="F24" s="5">
+        <v>100</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.497</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0.127</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.497</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
+        <v>100</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="5">
+        <v>100</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="I25" s="7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="L25" s="7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5">
+        <v>100</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
+        <v>7</v>
+      </c>
+      <c r="F26" s="5">
+        <v>100</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="I26" s="7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>100</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5">
+        <v>100</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="I27" s="7">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="M27" s="7">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5">
+        <v>100</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>15</v>
+      </c>
+      <c r="F28" s="5">
+        <v>100</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I28" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5">
+        <v>100</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
+        <v>20</v>
+      </c>
+      <c r="F29" s="5">
+        <v>100</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I29" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="M29" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5">
+        <v>100</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5">
+        <v>100</v>
+      </c>
+      <c r="H30" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I30" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K30" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="M30" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>100</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>50</v>
+      </c>
+      <c r="F31" s="5">
+        <v>100</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I31" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J31" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K31" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="M31" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5">
+        <v>100</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5">
+        <v>100</v>
+      </c>
+      <c r="F32" s="5">
+        <v>100</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I32" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J32" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="M32" s="7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5">
+        <v>100</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <v>150</v>
+      </c>
+      <c r="F33" s="5">
+        <v>100</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L33" s="7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0.995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made bar chart code my dynamic
</commit_message>
<xml_diff>
--- a/evidence/configurations.xlsx
+++ b/evidence/configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\F21DL-CW2\evidence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C6D40D-47C6-4DCC-AC23-705EB62D2FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A7F51-4877-453C-91AB-D3C8A170F9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14610" yWindow="4550" windowWidth="28800" windowHeight="13640" activeTab="1" xr2:uid="{87CF2611-45DB-404B-9ED3-045615C6A122}"/>
+    <workbookView xWindow="9600" yWindow="3010" windowWidth="28800" windowHeight="13640" activeTab="1" xr2:uid="{87CF2611-45DB-404B-9ED3-045615C6A122}"/>
   </bookViews>
   <sheets>
     <sheet name="J48" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Binary Splits</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Max Depth</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -3118,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BB2B9A-1435-4A52-9948-1AEE37B4D992}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4038,14 +4035,14 @@
       <c r="I24" s="7">
         <v>0.127</v>
       </c>
-      <c r="J24" s="7" t="s">
-        <v>17</v>
+      <c r="J24" s="7">
+        <v>0</v>
       </c>
       <c r="K24" s="7">
         <v>0.497</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>17</v>
+      <c r="L24" s="7">
+        <v>0</v>
       </c>
       <c r="M24" s="7">
         <v>0.85799999999999998</v>

</xml_diff>